<commit_message>
graficas arregladas, sigue panel corropletico y demas
</commit_message>
<xml_diff>
--- a/data/BalanceHidrico_Dashboard.xlsx
+++ b/data/BalanceHidrico_Dashboard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\c.segurab\Documents\DashBoard\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{390DABEE-0CBC-4D95-B2EF-4FC0BCE4E6A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F72B163A-5C93-404C-97D9-7CEE74094BB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{11150094-1AF8-482C-9061-8E57AC1C8E9B}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{11150094-1AF8-482C-9061-8E57AC1C8E9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -7790,34 +7790,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C2825AC-3A84-44E4-A53F-AE5A3054B116}">
   <dimension ref="A2:R50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D3" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" style="1"/>
-    <col min="5" max="5" width="14.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.88671875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5546875" style="1"/>
-    <col min="9" max="9" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5546875" style="1"/>
-    <col min="11" max="11" width="16.5546875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="21.5546875" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="11.5546875" style="1"/>
+    <col min="3" max="3" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" style="1"/>
+    <col min="5" max="5" width="14.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" style="1"/>
+    <col min="9" max="9" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" style="1"/>
+    <col min="11" max="11" width="16.5703125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="21.5703125" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
     </row>
-    <row r="3" spans="1:18" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -7866,7 +7866,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -7925,7 +7925,7 @@
         <v>3.4523824829558021</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -7984,7 +7984,7 @@
         <v>3.9911107265691652</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
@@ -8043,7 +8043,7 @@
         <v>4.0662366833211152</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
@@ -8102,7 +8102,7 @@
         <v>5.0041051288407372</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -8161,7 +8161,7 @@
         <v>3.9238596462237423</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
@@ -8220,7 +8220,7 @@
         <v>24.885198232081684</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
@@ -8279,7 +8279,7 @@
         <v>5.2756441219827748</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
@@ -8338,7 +8338,7 @@
         <v>-16.419770502675085</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
@@ -8397,7 +8397,7 @@
         <v>2.8566693902784341</v>
       </c>
     </row>
-    <row r="13" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <f>+[1]Validación!A14</f>
         <v>0</v>
@@ -8422,7 +8422,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="14" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <f>+[1]Validación!A15</f>
         <v>0</v>
@@ -8447,7 +8447,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="15" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
         <f>+[1]Validación!A16</f>
         <v>0</v>
@@ -8472,7 +8472,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>22</v>
       </c>
@@ -8531,7 +8531,7 @@
         <v>6.2580280509629613</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>23</v>
       </c>
@@ -8590,7 +8590,7 @@
         <v>9.1059407667986836</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>24</v>
       </c>
@@ -8649,7 +8649,7 @@
         <v>4.072309843943958</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>25</v>
       </c>
@@ -8708,7 +8708,7 @@
         <v>4.3288813356743283</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>26</v>
       </c>
@@ -8767,7 +8767,7 @@
         <v>6.377731662386533</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>27</v>
       </c>
@@ -8826,7 +8826,7 @@
         <v>1.7993618134211542</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>28</v>
       </c>
@@ -8885,7 +8885,7 @@
         <v>11.957309647981447</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>29</v>
       </c>
@@ -8944,7 +8944,7 @@
         <v>18.932144963358358</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>30</v>
       </c>
@@ -9003,7 +9003,7 @@
         <v>3.7907031733142675</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>31</v>
       </c>
@@ -9062,7 +9062,7 @@
         <v>6.6020853589625972</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>32</v>
       </c>
@@ -9121,7 +9121,7 @@
         <v>1.7533440385659127</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>33</v>
       </c>
@@ -9180,7 +9180,7 @@
         <v>19.085203764771357</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>34</v>
       </c>
@@ -9239,7 +9239,7 @@
         <v>9.2036086052323061</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>35</v>
       </c>
@@ -9298,7 +9298,7 @@
         <v>11.867685329352225</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>36</v>
       </c>
@@ -9357,7 +9357,7 @@
         <v>19.129445779534858</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>37</v>
       </c>
@@ -9416,7 +9416,7 @@
         <v>25.421090669256227</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>38</v>
       </c>
@@ -9475,7 +9475,7 @@
         <v>10.431387078529312</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>39</v>
       </c>
@@ -9534,7 +9534,7 @@
         <v>10.608040744651888</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>40</v>
       </c>
@@ -9593,7 +9593,7 @@
         <v>5.4693875529000717</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>41</v>
       </c>
@@ -9652,7 +9652,7 @@
         <v>10.276476854994796</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>42</v>
       </c>
@@ -9711,7 +9711,7 @@
         <v>19.778061075920569</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>43</v>
       </c>
@@ -9770,7 +9770,7 @@
         <v>16.262462635072001</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>44</v>
       </c>
@@ -9829,7 +9829,7 @@
         <v>4.3747611745606401</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>45</v>
       </c>
@@ -9888,7 +9888,7 @@
         <v>8.9215645197447131</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>46</v>
       </c>
@@ -9947,7 +9947,7 @@
         <v>13.195662801448595</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>47</v>
       </c>
@@ -10006,7 +10006,7 @@
         <v>23.874311655600586</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>48</v>
       </c>
@@ -10065,7 +10065,7 @@
         <v>28.926840833071122</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>49</v>
       </c>
@@ -10124,7 +10124,7 @@
         <v>8.1249431483813535</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>50</v>
       </c>
@@ -10183,7 +10183,7 @@
         <v>3.9786657159594578</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>51</v>
       </c>
@@ -10242,7 +10242,7 @@
         <v>4.7539747684474545</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>52</v>
       </c>
@@ -10301,7 +10301,7 @@
         <v>3.9147438723616301</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>53</v>
       </c>
@@ -10360,7 +10360,7 @@
         <v>9.5539868609884842</v>
       </c>
     </row>
-    <row r="49" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="49" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D49" s="5">
         <f>SUM(D4:D46)</f>
         <v>89.299740826669151</v>
@@ -10407,7 +10407,7 @@
         <v>6.0984662434789856</v>
       </c>
     </row>
-    <row r="50" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="50" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D50" s="5">
         <v>103.37090822113825</v>
       </c>

</xml_diff>